<commit_message>
Done with my task
</commit_message>
<xml_diff>
--- a/Updated backlog 27-02-2019.xlsx
+++ b/Updated backlog 27-02-2019.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\BI\6th Semester\Software Engineering\Project\KO7F\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
   <si>
     <t>User story</t>
   </si>
@@ -168,9 +173,6 @@
     <t>hazem tarek</t>
   </si>
   <si>
-    <t>arrousi</t>
-  </si>
-  <si>
     <t>1.9&amp;1.8</t>
   </si>
   <si>
@@ -190,12 +192,18 @@
   </si>
   <si>
     <t>omar khaled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can delete events </t>
+  </si>
+  <si>
+    <t>Omar Al Arousi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -322,15 +330,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:colOff>60960</xdr:colOff>
           <xdr:row>54</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>361950</xdr:colOff>
+          <xdr:colOff>365760</xdr:colOff>
           <xdr:row>55</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -343,7 +351,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -351,6 +359,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -363,15 +394,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:colOff>60960</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>361950</xdr:colOff>
+          <xdr:colOff>365760</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -384,7 +415,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -392,6 +423,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -404,15 +458,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:colOff>60960</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>361950</xdr:colOff>
+          <xdr:colOff>365760</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -425,7 +479,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -433,6 +487,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -486,7 +563,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,7 +598,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -732,26 +809,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="98.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="98.5546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -771,7 +848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -779,7 +856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.1000000000000001</v>
       </c>
@@ -793,7 +870,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.2</v>
       </c>
@@ -810,7 +887,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.3</v>
       </c>
@@ -827,7 +904,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1.4</v>
       </c>
@@ -844,7 +921,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1.5</v>
       </c>
@@ -855,10 +932,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1.6</v>
       </c>
@@ -869,10 +946,10 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1.7</v>
       </c>
@@ -886,10 +963,10 @@
         <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1.8</v>
       </c>
@@ -903,7 +980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1.9</v>
       </c>
@@ -917,10 +994,10 @@
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -934,7 +1011,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -942,7 +1019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>2.1</v>
       </c>
@@ -956,7 +1033,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -973,7 +1050,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -990,7 +1067,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>2.4</v>
       </c>
@@ -1007,7 +1084,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>2.5</v>
       </c>
@@ -1024,7 +1101,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>2.6</v>
       </c>
@@ -1041,7 +1118,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>2.7</v>
       </c>
@@ -1052,13 +1129,13 @@
         <v>5</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="4">
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>2.8</v>
       </c>
@@ -1072,7 +1149,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>2.9</v>
       </c>
@@ -1089,7 +1166,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>2.1</v>
       </c>
@@ -1106,7 +1183,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>2.11</v>
       </c>
@@ -1117,10 +1194,10 @@
         <v>5</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>2.12</v>
       </c>
@@ -1131,13 +1208,13 @@
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="4">
         <v>2.11</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>2.13</v>
       </c>
@@ -1148,10 +1225,10 @@
         <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>2.14</v>
       </c>
@@ -1162,16 +1239,16 @@
         <v>8</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="4">
         <v>2.11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>11</v>
       </c>
@@ -1179,7 +1256,7 @@
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1199,7 +1276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -1207,7 +1284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1.1000000000000001</v>
       </c>
@@ -1218,10 +1295,10 @@
         <v>5</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1.2</v>
       </c>
@@ -1232,13 +1309,13 @@
         <v>8</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E34" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1.3</v>
       </c>
@@ -1249,13 +1326,13 @@
         <v>5</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E35" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1.4</v>
       </c>
@@ -1266,10 +1343,10 @@
         <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1.5</v>
       </c>
@@ -1280,13 +1357,13 @@
         <v>8</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E37" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1.6</v>
       </c>
@@ -1297,10 +1374,10 @@
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1.7</v>
       </c>
@@ -1311,10 +1388,10 @@
         <v>8</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>2</v>
       </c>
@@ -1322,7 +1399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>2.1</v>
       </c>
@@ -1336,7 +1413,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -1353,7 +1430,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -1370,7 +1447,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2.4</v>
       </c>
@@ -1387,7 +1464,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2.5</v>
       </c>
@@ -1398,13 +1475,13 @@
         <v>5</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E45" s="4">
         <v>1.6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2.6</v>
       </c>
@@ -1415,13 +1492,13 @@
         <v>5</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E46" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2.7</v>
       </c>
@@ -1432,10 +1509,10 @@
         <v>8</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2.8</v>
       </c>
@@ -1446,10 +1523,10 @@
         <v>5</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2.9</v>
       </c>
@@ -1460,13 +1537,13 @@
         <v>8</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E49" s="4">
         <v>2.8</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>2.1</v>
       </c>
@@ -1477,10 +1554,10 @@
         <v>8</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2.11</v>
       </c>
@@ -1491,13 +1568,13 @@
         <v>5</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E51" s="3">
         <v>2.1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2.12</v>
       </c>
@@ -1508,298 +1585,312 @@
         <v>8</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E52" s="3">
         <v>2.1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>2.13</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="4">
+        <v>8</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -1831,15 +1922,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:colOff>60960</xdr:colOff>
                     <xdr:row>54</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>361950</xdr:colOff>
+                    <xdr:colOff>365760</xdr:colOff>
                     <xdr:row>55</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1853,15 +1944,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:colOff>60960</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>361950</xdr:colOff>
+                    <xdr:colOff>365760</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1875,15 +1966,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:colOff>60960</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>361950</xdr:colOff>
+                    <xdr:colOff>365760</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1902,7 +1993,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1914,7 +2005,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>